<commit_message>
4th commit on 23 Dec 2023
</commit_message>
<xml_diff>
--- a/_site/data/data.xlsx
+++ b/_site/data/data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yapinghuang/Desktop/Year 2024/macro/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8697932D-CAC4-294B-BFD8-C7A63FAAD59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103426F5-63ED-8342-B7BA-10D12E49F125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="3040" windowWidth="32920" windowHeight="16940" xr2:uid="{705E9BD4-3817-D147-920D-CA616DF44740}"/>
+    <workbookView xWindow="5500" yWindow="3040" windowWidth="38440" windowHeight="20560" activeTab="2" xr2:uid="{705E9BD4-3817-D147-920D-CA616DF44740}"/>
   </bookViews>
   <sheets>
-    <sheet name="UOM_CS" sheetId="1" r:id="rId1"/>
+    <sheet name="CPI (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="UOM_CS" sheetId="1" r:id="rId2"/>
+    <sheet name="CPI" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Actual</t>
   </si>
@@ -49,11 +51,20 @@
   <si>
     <t>Release_Date</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.0"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -120,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,6 +159,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,11 +477,2187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55F8C8C-8B63-124A-85B0-B8145A966819}">
+  <dimension ref="A1:B240"/>
+  <sheetViews>
+    <sheetView topLeftCell="A175" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193:XFD193"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12">
+        <v>37987</v>
+      </c>
+      <c r="B2" s="13">
+        <v>185.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="12">
+        <f>EDATE(A2, 1)</f>
+        <v>38018</v>
+      </c>
+      <c r="B3" s="13">
+        <v>186.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="12">
+        <f t="shared" ref="A4:A67" si="0">EDATE(A3, 1)</f>
+        <v>38047</v>
+      </c>
+      <c r="B4" s="13">
+        <v>187.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="12">
+        <f t="shared" si="0"/>
+        <v>38078</v>
+      </c>
+      <c r="B5" s="13">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="12">
+        <f t="shared" si="0"/>
+        <v>38108</v>
+      </c>
+      <c r="B6" s="13">
+        <v>189.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="12">
+        <f t="shared" si="0"/>
+        <v>38139</v>
+      </c>
+      <c r="B7" s="13">
+        <v>189.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12">
+        <f t="shared" si="0"/>
+        <v>38169</v>
+      </c>
+      <c r="B8" s="13">
+        <v>189.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12">
+        <f t="shared" si="0"/>
+        <v>38200</v>
+      </c>
+      <c r="B9" s="13">
+        <v>189.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12">
+        <f t="shared" si="0"/>
+        <v>38231</v>
+      </c>
+      <c r="B10" s="13">
+        <v>189.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12">
+        <f t="shared" si="0"/>
+        <v>38261</v>
+      </c>
+      <c r="B11" s="13">
+        <v>190.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12">
+        <f t="shared" si="0"/>
+        <v>38292</v>
+      </c>
+      <c r="B12" s="13">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="12">
+        <f t="shared" si="0"/>
+        <v>38322</v>
+      </c>
+      <c r="B13" s="13">
+        <v>190.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12">
+        <f t="shared" si="0"/>
+        <v>38353</v>
+      </c>
+      <c r="B14" s="13">
+        <v>190.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="12">
+        <f t="shared" si="0"/>
+        <v>38384</v>
+      </c>
+      <c r="B15" s="13">
+        <v>191.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="12">
+        <f t="shared" si="0"/>
+        <v>38412</v>
+      </c>
+      <c r="B16" s="13">
+        <v>193.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12">
+        <f t="shared" si="0"/>
+        <v>38443</v>
+      </c>
+      <c r="B17" s="13">
+        <v>194.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12">
+        <f t="shared" si="0"/>
+        <v>38473</v>
+      </c>
+      <c r="B18" s="13">
+        <v>194.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12">
+        <f t="shared" si="0"/>
+        <v>38504</v>
+      </c>
+      <c r="B19" s="13">
+        <v>194.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12">
+        <f t="shared" si="0"/>
+        <v>38534</v>
+      </c>
+      <c r="B20" s="13">
+        <v>195.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12">
+        <f t="shared" si="0"/>
+        <v>38565</v>
+      </c>
+      <c r="B21" s="13">
+        <v>196.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12">
+        <f t="shared" si="0"/>
+        <v>38596</v>
+      </c>
+      <c r="B22" s="13">
+        <v>198.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="12">
+        <f t="shared" si="0"/>
+        <v>38626</v>
+      </c>
+      <c r="B23" s="13">
+        <v>199.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12">
+        <f t="shared" si="0"/>
+        <v>38657</v>
+      </c>
+      <c r="B24" s="13">
+        <v>197.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="12">
+        <f t="shared" si="0"/>
+        <v>38687</v>
+      </c>
+      <c r="B25" s="13">
+        <v>196.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="12">
+        <f t="shared" si="0"/>
+        <v>38718</v>
+      </c>
+      <c r="B26" s="13">
+        <v>198.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="12">
+        <f t="shared" si="0"/>
+        <v>38749</v>
+      </c>
+      <c r="B27" s="13">
+        <v>198.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="12">
+        <f t="shared" si="0"/>
+        <v>38777</v>
+      </c>
+      <c r="B28" s="13">
+        <v>199.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="12">
+        <f t="shared" si="0"/>
+        <v>38808</v>
+      </c>
+      <c r="B29" s="13">
+        <v>201.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="12">
+        <f t="shared" si="0"/>
+        <v>38838</v>
+      </c>
+      <c r="B30" s="13">
+        <v>202.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="12">
+        <f t="shared" si="0"/>
+        <v>38869</v>
+      </c>
+      <c r="B31" s="13">
+        <v>202.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="12">
+        <f t="shared" si="0"/>
+        <v>38899</v>
+      </c>
+      <c r="B32" s="13">
+        <v>203.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="12">
+        <f t="shared" si="0"/>
+        <v>38930</v>
+      </c>
+      <c r="B33" s="13">
+        <v>203.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="12">
+        <f t="shared" si="0"/>
+        <v>38961</v>
+      </c>
+      <c r="B34" s="13">
+        <v>202.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="12">
+        <f t="shared" si="0"/>
+        <v>38991</v>
+      </c>
+      <c r="B35" s="13">
+        <v>201.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="12">
+        <f t="shared" si="0"/>
+        <v>39022</v>
+      </c>
+      <c r="B36" s="13">
+        <v>201.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="12">
+        <f t="shared" si="0"/>
+        <v>39052</v>
+      </c>
+      <c r="B37" s="13">
+        <v>201.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="12">
+        <f t="shared" si="0"/>
+        <v>39083</v>
+      </c>
+      <c r="B38" s="13">
+        <v>202.416</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="12">
+        <f t="shared" si="0"/>
+        <v>39114</v>
+      </c>
+      <c r="B39" s="13">
+        <v>203.499</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="12">
+        <f t="shared" si="0"/>
+        <v>39142</v>
+      </c>
+      <c r="B40" s="13">
+        <v>205.352</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="12">
+        <f t="shared" si="0"/>
+        <v>39173</v>
+      </c>
+      <c r="B41" s="13">
+        <v>206.68600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="12">
+        <f t="shared" si="0"/>
+        <v>39203</v>
+      </c>
+      <c r="B42" s="13">
+        <v>207.94900000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="12">
+        <f t="shared" si="0"/>
+        <v>39234</v>
+      </c>
+      <c r="B43" s="13">
+        <v>208.352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="12">
+        <f t="shared" si="0"/>
+        <v>39264</v>
+      </c>
+      <c r="B44" s="13">
+        <v>208.29900000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="12">
+        <f t="shared" si="0"/>
+        <v>39295</v>
+      </c>
+      <c r="B45" s="13">
+        <v>207.917</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="12">
+        <f t="shared" si="0"/>
+        <v>39326</v>
+      </c>
+      <c r="B46" s="13">
+        <v>208.49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="12">
+        <f t="shared" si="0"/>
+        <v>39356</v>
+      </c>
+      <c r="B47" s="13">
+        <v>208.93600000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="12">
+        <f t="shared" si="0"/>
+        <v>39387</v>
+      </c>
+      <c r="B48" s="13">
+        <v>210.17699999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="12">
+        <f t="shared" si="0"/>
+        <v>39417</v>
+      </c>
+      <c r="B49" s="13">
+        <v>210.036</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="12">
+        <f t="shared" si="0"/>
+        <v>39448</v>
+      </c>
+      <c r="B50" s="13">
+        <v>211.08</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="12">
+        <f t="shared" si="0"/>
+        <v>39479</v>
+      </c>
+      <c r="B51" s="13">
+        <v>211.69300000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="12">
+        <f t="shared" si="0"/>
+        <v>39508</v>
+      </c>
+      <c r="B52" s="13">
+        <v>213.52799999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="12">
+        <f t="shared" si="0"/>
+        <v>39539</v>
+      </c>
+      <c r="B53" s="13">
+        <v>214.82300000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="12">
+        <f t="shared" si="0"/>
+        <v>39569</v>
+      </c>
+      <c r="B54" s="13">
+        <v>216.63200000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="12">
+        <f t="shared" si="0"/>
+        <v>39600</v>
+      </c>
+      <c r="B55" s="13">
+        <v>218.815</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="12">
+        <f t="shared" si="0"/>
+        <v>39630</v>
+      </c>
+      <c r="B56" s="13">
+        <v>219.964</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="12">
+        <f t="shared" si="0"/>
+        <v>39661</v>
+      </c>
+      <c r="B57" s="13">
+        <v>219.08600000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="12">
+        <f t="shared" si="0"/>
+        <v>39692</v>
+      </c>
+      <c r="B58" s="13">
+        <v>218.78299999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="12">
+        <f t="shared" si="0"/>
+        <v>39722</v>
+      </c>
+      <c r="B59" s="13">
+        <v>216.57300000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="12">
+        <f t="shared" si="0"/>
+        <v>39753</v>
+      </c>
+      <c r="B60" s="13">
+        <v>212.42500000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="12">
+        <f t="shared" si="0"/>
+        <v>39783</v>
+      </c>
+      <c r="B61" s="13">
+        <v>210.22800000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="12">
+        <f t="shared" si="0"/>
+        <v>39814</v>
+      </c>
+      <c r="B62" s="13">
+        <v>211.143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="12">
+        <f t="shared" si="0"/>
+        <v>39845</v>
+      </c>
+      <c r="B63" s="13">
+        <v>212.19300000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="12">
+        <f t="shared" si="0"/>
+        <v>39873</v>
+      </c>
+      <c r="B64" s="13">
+        <v>212.709</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="12">
+        <f t="shared" si="0"/>
+        <v>39904</v>
+      </c>
+      <c r="B65" s="13">
+        <v>213.24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="12">
+        <f t="shared" si="0"/>
+        <v>39934</v>
+      </c>
+      <c r="B66" s="13">
+        <v>213.85599999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="12">
+        <f t="shared" si="0"/>
+        <v>39965</v>
+      </c>
+      <c r="B67" s="13">
+        <v>215.69300000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="12">
+        <f t="shared" ref="A68:A131" si="1">EDATE(A67, 1)</f>
+        <v>39995</v>
+      </c>
+      <c r="B68" s="13">
+        <v>215.351</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="12">
+        <f t="shared" si="1"/>
+        <v>40026</v>
+      </c>
+      <c r="B69" s="13">
+        <v>215.834</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="12">
+        <f t="shared" si="1"/>
+        <v>40057</v>
+      </c>
+      <c r="B70" s="13">
+        <v>215.96899999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="12">
+        <f t="shared" si="1"/>
+        <v>40087</v>
+      </c>
+      <c r="B71" s="13">
+        <v>216.17699999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="12">
+        <f t="shared" si="1"/>
+        <v>40118</v>
+      </c>
+      <c r="B72" s="13">
+        <v>216.33</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="12">
+        <f t="shared" si="1"/>
+        <v>40148</v>
+      </c>
+      <c r="B73" s="13">
+        <v>215.94900000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="12">
+        <f t="shared" si="1"/>
+        <v>40179</v>
+      </c>
+      <c r="B74" s="13">
+        <v>216.68700000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="12">
+        <f t="shared" si="1"/>
+        <v>40210</v>
+      </c>
+      <c r="B75" s="13">
+        <v>216.74100000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="12">
+        <f t="shared" si="1"/>
+        <v>40238</v>
+      </c>
+      <c r="B76" s="13">
+        <v>217.631</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="12">
+        <f t="shared" si="1"/>
+        <v>40269</v>
+      </c>
+      <c r="B77" s="13">
+        <v>218.00899999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="12">
+        <f t="shared" si="1"/>
+        <v>40299</v>
+      </c>
+      <c r="B78" s="13">
+        <v>218.178</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="12">
+        <f t="shared" si="1"/>
+        <v>40330</v>
+      </c>
+      <c r="B79" s="13">
+        <v>217.965</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="12">
+        <f t="shared" si="1"/>
+        <v>40360</v>
+      </c>
+      <c r="B80" s="13">
+        <v>218.011</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="12">
+        <f t="shared" si="1"/>
+        <v>40391</v>
+      </c>
+      <c r="B81" s="13">
+        <v>218.31200000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="12">
+        <f t="shared" si="1"/>
+        <v>40422</v>
+      </c>
+      <c r="B82" s="13">
+        <v>218.43899999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="12">
+        <f t="shared" si="1"/>
+        <v>40452</v>
+      </c>
+      <c r="B83" s="13">
+        <v>218.71100000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="12">
+        <f t="shared" si="1"/>
+        <v>40483</v>
+      </c>
+      <c r="B84" s="13">
+        <v>218.803</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="12">
+        <f t="shared" si="1"/>
+        <v>40513</v>
+      </c>
+      <c r="B85" s="13">
+        <v>219.179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="12">
+        <f t="shared" si="1"/>
+        <v>40544</v>
+      </c>
+      <c r="B86" s="13">
+        <v>220.22300000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="12">
+        <f t="shared" si="1"/>
+        <v>40575</v>
+      </c>
+      <c r="B87" s="13">
+        <v>221.309</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="12">
+        <f t="shared" si="1"/>
+        <v>40603</v>
+      </c>
+      <c r="B88" s="13">
+        <v>223.46700000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="12">
+        <f t="shared" si="1"/>
+        <v>40634</v>
+      </c>
+      <c r="B89" s="13">
+        <v>224.90600000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="12">
+        <f t="shared" si="1"/>
+        <v>40664</v>
+      </c>
+      <c r="B90" s="13">
+        <v>225.964</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="12">
+        <f t="shared" si="1"/>
+        <v>40695</v>
+      </c>
+      <c r="B91" s="13">
+        <v>225.72200000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="12">
+        <f t="shared" si="1"/>
+        <v>40725</v>
+      </c>
+      <c r="B92" s="13">
+        <v>225.922</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="12">
+        <f t="shared" si="1"/>
+        <v>40756</v>
+      </c>
+      <c r="B93" s="13">
+        <v>226.54499999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="12">
+        <f t="shared" si="1"/>
+        <v>40787</v>
+      </c>
+      <c r="B94" s="13">
+        <v>226.88900000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="12">
+        <f t="shared" si="1"/>
+        <v>40817</v>
+      </c>
+      <c r="B95" s="13">
+        <v>226.42099999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="12">
+        <f t="shared" si="1"/>
+        <v>40848</v>
+      </c>
+      <c r="B96" s="13">
+        <v>226.23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="12">
+        <f t="shared" si="1"/>
+        <v>40878</v>
+      </c>
+      <c r="B97" s="13">
+        <v>225.672</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="12">
+        <f t="shared" si="1"/>
+        <v>40909</v>
+      </c>
+      <c r="B98" s="13">
+        <v>226.66499999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="12">
+        <f t="shared" si="1"/>
+        <v>40940</v>
+      </c>
+      <c r="B99" s="13">
+        <v>227.66300000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="12">
+        <f t="shared" si="1"/>
+        <v>40969</v>
+      </c>
+      <c r="B100" s="13">
+        <v>229.392</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="12">
+        <f t="shared" si="1"/>
+        <v>41000</v>
+      </c>
+      <c r="B101" s="13">
+        <v>230.08500000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="12">
+        <f t="shared" si="1"/>
+        <v>41030</v>
+      </c>
+      <c r="B102" s="13">
+        <v>229.815</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="12">
+        <f t="shared" si="1"/>
+        <v>41061</v>
+      </c>
+      <c r="B103" s="13">
+        <v>229.47800000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="12">
+        <f t="shared" si="1"/>
+        <v>41091</v>
+      </c>
+      <c r="B104" s="13">
+        <v>229.10400000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="12">
+        <f t="shared" si="1"/>
+        <v>41122</v>
+      </c>
+      <c r="B105" s="13">
+        <v>230.37899999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="12">
+        <f t="shared" si="1"/>
+        <v>41153</v>
+      </c>
+      <c r="B106" s="13">
+        <v>231.40700000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="12">
+        <f t="shared" si="1"/>
+        <v>41183</v>
+      </c>
+      <c r="B107" s="13">
+        <v>231.31700000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="12">
+        <f t="shared" si="1"/>
+        <v>41214</v>
+      </c>
+      <c r="B108" s="13">
+        <v>230.221</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="12">
+        <f t="shared" si="1"/>
+        <v>41244</v>
+      </c>
+      <c r="B109" s="13">
+        <v>229.601</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="12">
+        <f t="shared" si="1"/>
+        <v>41275</v>
+      </c>
+      <c r="B110" s="13">
+        <v>230.28</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="12">
+        <f t="shared" si="1"/>
+        <v>41306</v>
+      </c>
+      <c r="B111" s="13">
+        <v>232.166</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="12">
+        <f t="shared" si="1"/>
+        <v>41334</v>
+      </c>
+      <c r="B112" s="13">
+        <v>232.773</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="12">
+        <f t="shared" si="1"/>
+        <v>41365</v>
+      </c>
+      <c r="B113" s="13">
+        <v>232.53100000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="12">
+        <f t="shared" si="1"/>
+        <v>41395</v>
+      </c>
+      <c r="B114" s="13">
+        <v>232.94499999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="12">
+        <f t="shared" si="1"/>
+        <v>41426</v>
+      </c>
+      <c r="B115" s="13">
+        <v>233.50399999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="12">
+        <f t="shared" si="1"/>
+        <v>41456</v>
+      </c>
+      <c r="B116" s="13">
+        <v>233.596</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="12">
+        <f t="shared" si="1"/>
+        <v>41487</v>
+      </c>
+      <c r="B117" s="13">
+        <v>233.87700000000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="12">
+        <f t="shared" si="1"/>
+        <v>41518</v>
+      </c>
+      <c r="B118" s="13">
+        <v>234.149</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="12">
+        <f t="shared" si="1"/>
+        <v>41548</v>
+      </c>
+      <c r="B119" s="13">
+        <v>233.54599999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="12">
+        <f t="shared" si="1"/>
+        <v>41579</v>
+      </c>
+      <c r="B120" s="13">
+        <v>233.06899999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="12">
+        <f t="shared" si="1"/>
+        <v>41609</v>
+      </c>
+      <c r="B121" s="13">
+        <v>233.04900000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="12">
+        <f t="shared" si="1"/>
+        <v>41640</v>
+      </c>
+      <c r="B122" s="13">
+        <v>233.916</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="12">
+        <f t="shared" si="1"/>
+        <v>41671</v>
+      </c>
+      <c r="B123" s="13">
+        <v>234.78100000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="12">
+        <f t="shared" si="1"/>
+        <v>41699</v>
+      </c>
+      <c r="B124" s="13">
+        <v>236.29300000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="12">
+        <f t="shared" si="1"/>
+        <v>41730</v>
+      </c>
+      <c r="B125" s="13">
+        <v>237.072</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="12">
+        <f t="shared" si="1"/>
+        <v>41760</v>
+      </c>
+      <c r="B126" s="13">
+        <v>237.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="12">
+        <f t="shared" si="1"/>
+        <v>41791</v>
+      </c>
+      <c r="B127" s="13">
+        <v>238.34299999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="12">
+        <f t="shared" si="1"/>
+        <v>41821</v>
+      </c>
+      <c r="B128" s="13">
+        <v>238.25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="12">
+        <f t="shared" si="1"/>
+        <v>41852</v>
+      </c>
+      <c r="B129" s="13">
+        <v>237.852</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="12">
+        <f t="shared" si="1"/>
+        <v>41883</v>
+      </c>
+      <c r="B130" s="13">
+        <v>238.03100000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="12">
+        <f t="shared" si="1"/>
+        <v>41913</v>
+      </c>
+      <c r="B131" s="13">
+        <v>237.43299999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="12">
+        <f t="shared" ref="A132:A195" si="2">EDATE(A131, 1)</f>
+        <v>41944</v>
+      </c>
+      <c r="B132" s="13">
+        <v>236.15100000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="12">
+        <f t="shared" si="2"/>
+        <v>41974</v>
+      </c>
+      <c r="B133" s="13">
+        <v>234.81200000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="12">
+        <f t="shared" si="2"/>
+        <v>42005</v>
+      </c>
+      <c r="B134" s="13">
+        <v>233.70699999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="12">
+        <f t="shared" si="2"/>
+        <v>42036</v>
+      </c>
+      <c r="B135" s="13">
+        <v>234.72200000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="12">
+        <f t="shared" si="2"/>
+        <v>42064</v>
+      </c>
+      <c r="B136" s="13">
+        <v>236.119</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="12">
+        <f t="shared" si="2"/>
+        <v>42095</v>
+      </c>
+      <c r="B137" s="13">
+        <v>236.59899999999999</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="12">
+        <f t="shared" si="2"/>
+        <v>42125</v>
+      </c>
+      <c r="B138" s="13">
+        <v>237.80500000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="12">
+        <f t="shared" si="2"/>
+        <v>42156</v>
+      </c>
+      <c r="B139" s="13">
+        <v>238.63800000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="12">
+        <f t="shared" si="2"/>
+        <v>42186</v>
+      </c>
+      <c r="B140" s="13">
+        <v>238.654</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="12">
+        <f t="shared" si="2"/>
+        <v>42217</v>
+      </c>
+      <c r="B141" s="13">
+        <v>238.316</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="12">
+        <f t="shared" si="2"/>
+        <v>42248</v>
+      </c>
+      <c r="B142" s="13">
+        <v>237.94499999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="12">
+        <f t="shared" si="2"/>
+        <v>42278</v>
+      </c>
+      <c r="B143" s="13">
+        <v>237.83799999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="12">
+        <f t="shared" si="2"/>
+        <v>42309</v>
+      </c>
+      <c r="B144" s="13">
+        <v>237.33600000000001</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="12">
+        <f t="shared" si="2"/>
+        <v>42339</v>
+      </c>
+      <c r="B145" s="13">
+        <v>236.52500000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="12">
+        <f t="shared" si="2"/>
+        <v>42370</v>
+      </c>
+      <c r="B146" s="13">
+        <v>236.916</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="12">
+        <f t="shared" si="2"/>
+        <v>42401</v>
+      </c>
+      <c r="B147" s="13">
+        <v>237.11099999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="12">
+        <f t="shared" si="2"/>
+        <v>42430</v>
+      </c>
+      <c r="B148" s="13">
+        <v>238.13200000000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="12">
+        <f t="shared" si="2"/>
+        <v>42461</v>
+      </c>
+      <c r="B149" s="13">
+        <v>239.261</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="12">
+        <f t="shared" si="2"/>
+        <v>42491</v>
+      </c>
+      <c r="B150" s="13">
+        <v>240.22900000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="12">
+        <f t="shared" si="2"/>
+        <v>42522</v>
+      </c>
+      <c r="B151" s="13">
+        <v>241.018</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="12">
+        <f t="shared" si="2"/>
+        <v>42552</v>
+      </c>
+      <c r="B152" s="13">
+        <v>240.62799999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="12">
+        <f t="shared" si="2"/>
+        <v>42583</v>
+      </c>
+      <c r="B153" s="13">
+        <v>240.84899999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="12">
+        <f t="shared" si="2"/>
+        <v>42614</v>
+      </c>
+      <c r="B154" s="13">
+        <v>241.428</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="12">
+        <f t="shared" si="2"/>
+        <v>42644</v>
+      </c>
+      <c r="B155" s="13">
+        <v>241.72900000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="12">
+        <f t="shared" si="2"/>
+        <v>42675</v>
+      </c>
+      <c r="B156" s="13">
+        <v>241.35300000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="12">
+        <f t="shared" si="2"/>
+        <v>42705</v>
+      </c>
+      <c r="B157" s="13">
+        <v>241.43199999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="12">
+        <f t="shared" si="2"/>
+        <v>42736</v>
+      </c>
+      <c r="B158" s="13">
+        <v>242.839</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="12">
+        <f t="shared" si="2"/>
+        <v>42767</v>
+      </c>
+      <c r="B159" s="13">
+        <v>243.60300000000001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="12">
+        <f t="shared" si="2"/>
+        <v>42795</v>
+      </c>
+      <c r="B160" s="13">
+        <v>243.80099999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="12">
+        <f t="shared" si="2"/>
+        <v>42826</v>
+      </c>
+      <c r="B161" s="13">
+        <v>244.524</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="12">
+        <f t="shared" si="2"/>
+        <v>42856</v>
+      </c>
+      <c r="B162" s="13">
+        <v>244.733</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="12">
+        <f t="shared" si="2"/>
+        <v>42887</v>
+      </c>
+      <c r="B163" s="13">
+        <v>244.95500000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="12">
+        <f t="shared" si="2"/>
+        <v>42917</v>
+      </c>
+      <c r="B164" s="13">
+        <v>244.786</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="12">
+        <f t="shared" si="2"/>
+        <v>42948</v>
+      </c>
+      <c r="B165" s="13">
+        <v>245.51900000000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" s="12">
+        <f t="shared" si="2"/>
+        <v>42979</v>
+      </c>
+      <c r="B166" s="13">
+        <v>246.81899999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="12">
+        <f t="shared" si="2"/>
+        <v>43009</v>
+      </c>
+      <c r="B167" s="13">
+        <v>246.66300000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" s="12">
+        <f t="shared" si="2"/>
+        <v>43040</v>
+      </c>
+      <c r="B168" s="13">
+        <v>246.66900000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" s="12">
+        <f t="shared" si="2"/>
+        <v>43070</v>
+      </c>
+      <c r="B169" s="13">
+        <v>246.524</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" s="12">
+        <f t="shared" si="2"/>
+        <v>43101</v>
+      </c>
+      <c r="B170" s="13">
+        <v>247.86699999999999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="12">
+        <f t="shared" si="2"/>
+        <v>43132</v>
+      </c>
+      <c r="B171" s="13">
+        <v>248.99100000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="12">
+        <f t="shared" si="2"/>
+        <v>43160</v>
+      </c>
+      <c r="B172" s="13">
+        <v>249.554</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" s="12">
+        <f t="shared" si="2"/>
+        <v>43191</v>
+      </c>
+      <c r="B173" s="13">
+        <v>250.54599999999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="12">
+        <f t="shared" si="2"/>
+        <v>43221</v>
+      </c>
+      <c r="B174" s="13">
+        <v>251.58799999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" s="12">
+        <f t="shared" si="2"/>
+        <v>43252</v>
+      </c>
+      <c r="B175" s="13">
+        <v>251.989</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" s="12">
+        <f t="shared" si="2"/>
+        <v>43282</v>
+      </c>
+      <c r="B176" s="13">
+        <v>252.006</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" s="12">
+        <f t="shared" si="2"/>
+        <v>43313</v>
+      </c>
+      <c r="B177" s="13">
+        <v>252.14599999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="12">
+        <f t="shared" si="2"/>
+        <v>43344</v>
+      </c>
+      <c r="B178" s="13">
+        <v>252.43899999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="12">
+        <f t="shared" si="2"/>
+        <v>43374</v>
+      </c>
+      <c r="B179" s="13">
+        <v>252.88499999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" s="12">
+        <f t="shared" si="2"/>
+        <v>43405</v>
+      </c>
+      <c r="B180" s="13">
+        <v>252.03800000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" s="12">
+        <f t="shared" si="2"/>
+        <v>43435</v>
+      </c>
+      <c r="B181" s="13">
+        <v>251.233</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" s="12">
+        <f t="shared" si="2"/>
+        <v>43466</v>
+      </c>
+      <c r="B182" s="13">
+        <v>251.71199999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" s="12">
+        <f t="shared" si="2"/>
+        <v>43497</v>
+      </c>
+      <c r="B183" s="13">
+        <v>252.77600000000001</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" s="12">
+        <f t="shared" si="2"/>
+        <v>43525</v>
+      </c>
+      <c r="B184" s="13">
+        <v>254.202</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="12">
+        <f t="shared" si="2"/>
+        <v>43556</v>
+      </c>
+      <c r="B185" s="13">
+        <v>255.548</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="12">
+        <f t="shared" si="2"/>
+        <v>43586</v>
+      </c>
+      <c r="B186" s="13">
+        <v>256.09199999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" s="12">
+        <f t="shared" si="2"/>
+        <v>43617</v>
+      </c>
+      <c r="B187" s="13">
+        <v>256.14299999999997</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="12">
+        <f t="shared" si="2"/>
+        <v>43647</v>
+      </c>
+      <c r="B188" s="13">
+        <v>256.57100000000003</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" s="12">
+        <f t="shared" si="2"/>
+        <v>43678</v>
+      </c>
+      <c r="B189" s="13">
+        <v>256.55799999999999</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" s="12">
+        <f t="shared" si="2"/>
+        <v>43709</v>
+      </c>
+      <c r="B190" s="13">
+        <v>256.75900000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" s="12">
+        <f t="shared" si="2"/>
+        <v>43739</v>
+      </c>
+      <c r="B191" s="13">
+        <v>257.346</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" s="12">
+        <f t="shared" si="2"/>
+        <v>43770</v>
+      </c>
+      <c r="B192" s="13">
+        <v>257.20800000000003</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" s="12">
+        <f t="shared" si="2"/>
+        <v>43800</v>
+      </c>
+      <c r="B193" s="13">
+        <v>256.97399999999999</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" s="12">
+        <f t="shared" si="2"/>
+        <v>43831</v>
+      </c>
+      <c r="B194" s="13">
+        <v>257.971</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" s="12">
+        <f t="shared" si="2"/>
+        <v>43862</v>
+      </c>
+      <c r="B195" s="13">
+        <v>258.678</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" s="12">
+        <f t="shared" ref="A196:A240" si="3">EDATE(A195, 1)</f>
+        <v>43891</v>
+      </c>
+      <c r="B196" s="13">
+        <v>258.11500000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" s="12">
+        <f t="shared" si="3"/>
+        <v>43922</v>
+      </c>
+      <c r="B197" s="13">
+        <v>256.38900000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" s="12">
+        <f t="shared" si="3"/>
+        <v>43952</v>
+      </c>
+      <c r="B198" s="13">
+        <v>256.39400000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" s="12">
+        <f t="shared" si="3"/>
+        <v>43983</v>
+      </c>
+      <c r="B199" s="13">
+        <v>257.79700000000003</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" s="12">
+        <f t="shared" si="3"/>
+        <v>44013</v>
+      </c>
+      <c r="B200" s="13">
+        <v>259.101</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" s="12">
+        <f t="shared" si="3"/>
+        <v>44044</v>
+      </c>
+      <c r="B201" s="13">
+        <v>259.91800000000001</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" s="12">
+        <f t="shared" si="3"/>
+        <v>44075</v>
+      </c>
+      <c r="B202" s="13">
+        <v>260.27999999999997</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" s="12">
+        <f t="shared" si="3"/>
+        <v>44105</v>
+      </c>
+      <c r="B203" s="13">
+        <v>260.38799999999998</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" s="12">
+        <f t="shared" si="3"/>
+        <v>44136</v>
+      </c>
+      <c r="B204" s="13">
+        <v>260.22899999999998</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" s="12">
+        <f t="shared" si="3"/>
+        <v>44166</v>
+      </c>
+      <c r="B205" s="13">
+        <v>260.47399999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" s="12">
+        <f t="shared" si="3"/>
+        <v>44197</v>
+      </c>
+      <c r="B206" s="13">
+        <v>261.58199999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" s="12">
+        <f t="shared" si="3"/>
+        <v>44228</v>
+      </c>
+      <c r="B207" s="13">
+        <v>263.01400000000001</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" s="12">
+        <f t="shared" si="3"/>
+        <v>44256</v>
+      </c>
+      <c r="B208" s="13">
+        <v>264.87700000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" s="12">
+        <f t="shared" si="3"/>
+        <v>44287</v>
+      </c>
+      <c r="B209" s="13">
+        <v>267.05399999999997</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" s="12">
+        <f t="shared" si="3"/>
+        <v>44317</v>
+      </c>
+      <c r="B210" s="13">
+        <v>269.19499999999999</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" s="12">
+        <f t="shared" si="3"/>
+        <v>44348</v>
+      </c>
+      <c r="B211" s="13">
+        <v>271.69600000000003</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" s="12">
+        <f t="shared" si="3"/>
+        <v>44378</v>
+      </c>
+      <c r="B212" s="13">
+        <v>273.00299999999999</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" s="12">
+        <f t="shared" si="3"/>
+        <v>44409</v>
+      </c>
+      <c r="B213" s="13">
+        <v>273.56700000000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" s="12">
+        <f t="shared" si="3"/>
+        <v>44440</v>
+      </c>
+      <c r="B214" s="13">
+        <v>274.31</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2">
+      <c r="A215" s="12">
+        <f t="shared" si="3"/>
+        <v>44470</v>
+      </c>
+      <c r="B215" s="13">
+        <v>276.589</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" s="12">
+        <f t="shared" si="3"/>
+        <v>44501</v>
+      </c>
+      <c r="B216" s="13">
+        <v>277.94799999999998</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" s="12">
+        <f t="shared" si="3"/>
+        <v>44531</v>
+      </c>
+      <c r="B217" s="13">
+        <v>278.80200000000002</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" s="12">
+        <f t="shared" si="3"/>
+        <v>44562</v>
+      </c>
+      <c r="B218" s="13">
+        <v>281.14800000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" s="12">
+        <f t="shared" si="3"/>
+        <v>44593</v>
+      </c>
+      <c r="B219" s="13">
+        <v>283.71600000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" s="12">
+        <f t="shared" si="3"/>
+        <v>44621</v>
+      </c>
+      <c r="B220" s="13">
+        <v>287.50400000000002</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" s="12">
+        <f t="shared" si="3"/>
+        <v>44652</v>
+      </c>
+      <c r="B221" s="13">
+        <v>289.10899999999998</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" s="12">
+        <f t="shared" si="3"/>
+        <v>44682</v>
+      </c>
+      <c r="B222" s="13">
+        <v>292.29599999999999</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" s="12">
+        <f t="shared" si="3"/>
+        <v>44713</v>
+      </c>
+      <c r="B223" s="13">
+        <v>296.31099999999998</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" s="12">
+        <f t="shared" si="3"/>
+        <v>44743</v>
+      </c>
+      <c r="B224" s="13">
+        <v>296.27600000000001</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" s="12">
+        <f t="shared" si="3"/>
+        <v>44774</v>
+      </c>
+      <c r="B225" s="13">
+        <v>296.17099999999999</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" s="12">
+        <f t="shared" si="3"/>
+        <v>44805</v>
+      </c>
+      <c r="B226" s="13">
+        <v>296.80799999999999</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" s="12">
+        <f t="shared" si="3"/>
+        <v>44835</v>
+      </c>
+      <c r="B227" s="13">
+        <v>298.012</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" s="12">
+        <f t="shared" si="3"/>
+        <v>44866</v>
+      </c>
+      <c r="B228" s="13">
+        <v>297.71100000000001</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="A229" s="12">
+        <f t="shared" si="3"/>
+        <v>44896</v>
+      </c>
+      <c r="B229" s="13">
+        <v>296.79700000000003</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" s="12">
+        <f t="shared" si="3"/>
+        <v>44927</v>
+      </c>
+      <c r="B230" s="13">
+        <v>299.17</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" s="12">
+        <f t="shared" si="3"/>
+        <v>44958</v>
+      </c>
+      <c r="B231" s="13">
+        <v>300.83999999999997</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" s="12">
+        <f t="shared" si="3"/>
+        <v>44986</v>
+      </c>
+      <c r="B232" s="13">
+        <v>301.83600000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" s="12">
+        <f t="shared" si="3"/>
+        <v>45017</v>
+      </c>
+      <c r="B233" s="13">
+        <v>303.363</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" s="12">
+        <f t="shared" si="3"/>
+        <v>45047</v>
+      </c>
+      <c r="B234" s="13">
+        <v>304.12700000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" s="12">
+        <f t="shared" si="3"/>
+        <v>45078</v>
+      </c>
+      <c r="B235" s="13">
+        <v>305.10899999999998</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" s="12">
+        <f t="shared" si="3"/>
+        <v>45108</v>
+      </c>
+      <c r="B236" s="13">
+        <v>305.69099999999997</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" s="12">
+        <f t="shared" si="3"/>
+        <v>45139</v>
+      </c>
+      <c r="B237" s="13">
+        <v>307.02600000000001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" s="12">
+        <f t="shared" si="3"/>
+        <v>45170</v>
+      </c>
+      <c r="B238" s="13">
+        <v>307.78899999999999</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" s="12">
+        <f t="shared" si="3"/>
+        <v>45200</v>
+      </c>
+      <c r="B239" s="13">
+        <v>307.67099999999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" s="12">
+        <f t="shared" si="3"/>
+        <v>45231</v>
+      </c>
+      <c r="B240" s="13">
+        <v>307.05099999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E3135A-89C8-594C-B704-4E64E6E6D914}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1435,7 +3627,7 @@
       </c>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:8">
       <c r="A65" s="3">
         <v>44330</v>
       </c>
@@ -1450,7 +3642,7 @@
       </c>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:8">
       <c r="A66" s="3">
         <v>44316</v>
       </c>
@@ -1465,7 +3657,7 @@
       </c>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:8">
       <c r="A67" s="3">
         <v>44302</v>
       </c>
@@ -1480,7 +3672,7 @@
       </c>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:8">
       <c r="A68" s="3">
         <v>44281</v>
       </c>
@@ -1495,7 +3687,7 @@
       </c>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:8">
       <c r="A69" s="3">
         <v>44267</v>
       </c>
@@ -1510,7 +3702,7 @@
       </c>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:8">
       <c r="A70" s="3">
         <v>44253</v>
       </c>
@@ -1525,7 +3717,7 @@
       </c>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:8">
       <c r="A71" s="3">
         <v>44239</v>
       </c>
@@ -1540,7 +3732,7 @@
       </c>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:8">
       <c r="A72" s="3">
         <v>44225</v>
       </c>
@@ -1555,7 +3747,7 @@
       </c>
       <c r="E72" s="2"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:8">
       <c r="A73" s="3">
         <v>44211</v>
       </c>
@@ -1570,7 +3762,7 @@
       </c>
       <c r="E73" s="2"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:8">
       <c r="A74" s="3">
         <v>44188</v>
       </c>
@@ -1584,8 +3776,9 @@
         <v>76.900000000000006</v>
       </c>
       <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="H74" s="11"/>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="3">
         <v>44176</v>
       </c>
@@ -1600,7 +3793,7 @@
       </c>
       <c r="E75" s="2"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:8">
       <c r="A76" s="3">
         <v>44160</v>
       </c>
@@ -1615,7 +3808,7 @@
       </c>
       <c r="E76" s="2"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:8">
       <c r="A77" s="3">
         <v>44148</v>
       </c>
@@ -1630,7 +3823,7 @@
       </c>
       <c r="E77" s="2"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:8">
       <c r="A78" s="3">
         <v>44134</v>
       </c>
@@ -1645,7 +3838,7 @@
       </c>
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:8">
       <c r="A79" s="3">
         <v>44120</v>
       </c>
@@ -1660,7 +3853,7 @@
       </c>
       <c r="E79" s="2"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:8">
       <c r="A80" s="3">
         <v>44106</v>
       </c>
@@ -2379,6 +4572,454 @@
         <v>100.1</v>
       </c>
       <c r="E127" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6037937-942E-FF41-ABE4-7E743CFAB7BE}">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="12">
+        <v>43831</v>
+      </c>
+      <c r="B2" s="13">
+        <v>257.971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="12">
+        <f t="shared" ref="A3" si="0">EDATE(A2, 1)</f>
+        <v>43862</v>
+      </c>
+      <c r="B3" s="13">
+        <v>258.678</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="12">
+        <f t="shared" ref="A4:A48" si="1">EDATE(A3, 1)</f>
+        <v>43891</v>
+      </c>
+      <c r="B4" s="13">
+        <v>258.11500000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="12">
+        <f t="shared" si="1"/>
+        <v>43922</v>
+      </c>
+      <c r="B5" s="13">
+        <v>256.38900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="12">
+        <f t="shared" si="1"/>
+        <v>43952</v>
+      </c>
+      <c r="B6" s="13">
+        <v>256.39400000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="12">
+        <f t="shared" si="1"/>
+        <v>43983</v>
+      </c>
+      <c r="B7" s="13">
+        <v>257.79700000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="12">
+        <f t="shared" si="1"/>
+        <v>44013</v>
+      </c>
+      <c r="B8" s="13">
+        <v>259.101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="12">
+        <f t="shared" si="1"/>
+        <v>44044</v>
+      </c>
+      <c r="B9" s="13">
+        <v>259.91800000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="12">
+        <f t="shared" si="1"/>
+        <v>44075</v>
+      </c>
+      <c r="B10" s="13">
+        <v>260.27999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="12">
+        <f t="shared" si="1"/>
+        <v>44105</v>
+      </c>
+      <c r="B11" s="13">
+        <v>260.38799999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12">
+        <f t="shared" si="1"/>
+        <v>44136</v>
+      </c>
+      <c r="B12" s="13">
+        <v>260.22899999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="12">
+        <f t="shared" si="1"/>
+        <v>44166</v>
+      </c>
+      <c r="B13" s="13">
+        <v>260.47399999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12">
+        <f t="shared" si="1"/>
+        <v>44197</v>
+      </c>
+      <c r="B14" s="13">
+        <v>261.58199999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="12">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B15" s="13">
+        <v>263.01400000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="12">
+        <f t="shared" si="1"/>
+        <v>44256</v>
+      </c>
+      <c r="B16" s="13">
+        <v>264.87700000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12">
+        <f t="shared" si="1"/>
+        <v>44287</v>
+      </c>
+      <c r="B17" s="13">
+        <v>267.05399999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12">
+        <f t="shared" si="1"/>
+        <v>44317</v>
+      </c>
+      <c r="B18" s="13">
+        <v>269.19499999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12">
+        <f t="shared" si="1"/>
+        <v>44348</v>
+      </c>
+      <c r="B19" s="13">
+        <v>271.69600000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12">
+        <f t="shared" si="1"/>
+        <v>44378</v>
+      </c>
+      <c r="B20" s="13">
+        <v>273.00299999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="12">
+        <f t="shared" si="1"/>
+        <v>44409</v>
+      </c>
+      <c r="B21" s="13">
+        <v>273.56700000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="12">
+        <f t="shared" si="1"/>
+        <v>44440</v>
+      </c>
+      <c r="B22" s="13">
+        <v>274.31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="12">
+        <f t="shared" si="1"/>
+        <v>44470</v>
+      </c>
+      <c r="B23" s="13">
+        <v>276.589</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="12">
+        <f t="shared" si="1"/>
+        <v>44501</v>
+      </c>
+      <c r="B24" s="13">
+        <v>277.94799999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="12">
+        <f t="shared" si="1"/>
+        <v>44531</v>
+      </c>
+      <c r="B25" s="13">
+        <v>278.80200000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="12">
+        <f t="shared" si="1"/>
+        <v>44562</v>
+      </c>
+      <c r="B26" s="13">
+        <v>281.14800000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="12">
+        <f t="shared" si="1"/>
+        <v>44593</v>
+      </c>
+      <c r="B27" s="13">
+        <v>283.71600000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="12">
+        <f t="shared" si="1"/>
+        <v>44621</v>
+      </c>
+      <c r="B28" s="13">
+        <v>287.50400000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="12">
+        <f t="shared" si="1"/>
+        <v>44652</v>
+      </c>
+      <c r="B29" s="13">
+        <v>289.10899999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="12">
+        <f t="shared" si="1"/>
+        <v>44682</v>
+      </c>
+      <c r="B30" s="13">
+        <v>292.29599999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="12">
+        <f t="shared" si="1"/>
+        <v>44713</v>
+      </c>
+      <c r="B31" s="13">
+        <v>296.31099999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="12">
+        <f t="shared" si="1"/>
+        <v>44743</v>
+      </c>
+      <c r="B32" s="13">
+        <v>296.27600000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="12">
+        <f t="shared" si="1"/>
+        <v>44774</v>
+      </c>
+      <c r="B33" s="13">
+        <v>296.17099999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="12">
+        <f t="shared" si="1"/>
+        <v>44805</v>
+      </c>
+      <c r="B34" s="13">
+        <v>296.80799999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="12">
+        <f t="shared" si="1"/>
+        <v>44835</v>
+      </c>
+      <c r="B35" s="13">
+        <v>298.012</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="12">
+        <f t="shared" si="1"/>
+        <v>44866</v>
+      </c>
+      <c r="B36" s="13">
+        <v>297.71100000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="12">
+        <f t="shared" si="1"/>
+        <v>44896</v>
+      </c>
+      <c r="B37" s="13">
+        <v>296.79700000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="12">
+        <f t="shared" si="1"/>
+        <v>44927</v>
+      </c>
+      <c r="B38" s="13">
+        <v>299.17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="12">
+        <f t="shared" si="1"/>
+        <v>44958</v>
+      </c>
+      <c r="B39" s="13">
+        <v>300.83999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="12">
+        <f t="shared" si="1"/>
+        <v>44986</v>
+      </c>
+      <c r="B40" s="13">
+        <v>301.83600000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="12">
+        <f t="shared" si="1"/>
+        <v>45017</v>
+      </c>
+      <c r="B41" s="13">
+        <v>303.363</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="12">
+        <f t="shared" si="1"/>
+        <v>45047</v>
+      </c>
+      <c r="B42" s="13">
+        <v>304.12700000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="12">
+        <f t="shared" si="1"/>
+        <v>45078</v>
+      </c>
+      <c r="B43" s="13">
+        <v>305.10899999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="12">
+        <f t="shared" si="1"/>
+        <v>45108</v>
+      </c>
+      <c r="B44" s="13">
+        <v>305.69099999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="12">
+        <f t="shared" si="1"/>
+        <v>45139</v>
+      </c>
+      <c r="B45" s="13">
+        <v>307.02600000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="12">
+        <f t="shared" si="1"/>
+        <v>45170</v>
+      </c>
+      <c r="B46" s="13">
+        <v>307.78899999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="12">
+        <f t="shared" si="1"/>
+        <v>45200</v>
+      </c>
+      <c r="B47" s="13">
+        <v>307.67099999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="12">
+        <f t="shared" si="1"/>
+        <v>45231</v>
+      </c>
+      <c r="B48" s="13">
+        <v>307.05099999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>